<commit_message>
Timetable & format update
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Side_Projects\TimeTableBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A092D-5471-4A75-B545-F8F9D712FB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EFA687-08D9-4A7B-BDBD-82FE00DDB973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B6DA0D74-3629-46E5-9D8D-82ECD94FA4ED}"/>
   </bookViews>
@@ -718,7 +718,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>